<commit_message>
solved the scrollbar in QPage
</commit_message>
<xml_diff>
--- a/data/customers.xlsx
+++ b/data/customers.xlsx
@@ -1,118 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\tkinter\Auto_Quote\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13335" windowHeight="10455"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="13335" windowHeight="10455" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
-  <si>
-    <t>公司名稱</t>
-  </si>
-  <si>
-    <t>統編</t>
-  </si>
-  <si>
-    <t>公司地址</t>
-  </si>
-  <si>
-    <t>聯絡人</t>
-  </si>
-  <si>
-    <t>聯絡電話</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>sdfsdffd</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>98745631</t>
-  </si>
-  <si>
-    <t>測試</t>
-  </si>
-  <si>
-    <t>1232456</t>
-  </si>
-  <si>
-    <t>測試地址</t>
-  </si>
-  <si>
-    <t>測試人</t>
-  </si>
-  <si>
-    <t>123487896545</t>
-  </si>
-  <si>
-    <t>測試12</t>
-  </si>
-  <si>
-    <t>987465632</t>
-  </si>
-  <si>
-    <t>測試1地址</t>
-  </si>
-  <si>
-    <t>測試人1</t>
-  </si>
-  <si>
-    <t>963258741</t>
-  </si>
-  <si>
-    <t>測試23</t>
-  </si>
-  <si>
-    <t>測試23地址</t>
-  </si>
-  <si>
-    <t>測試人23</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="新細明體"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="新細明體"/>
+      <charset val="136"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -131,21 +53,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -433,110 +414,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col width="10.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="10.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="8.140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="14.140625" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>公司名稱</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>統編</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>公司地址</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>聯絡人</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>聯絡電話</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sdfsdffd</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>98745631</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>測試</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1232456</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>測試地址</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>測試人</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>123487896545</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>測試12456</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>987465632</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>測試1地址</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>測試人1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>963258741</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sfsdfsd</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>sdfdsf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sdfsdf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sdfwef</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ewfefsdfs</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>